<commit_message>
R-MAT benchmark on Stampede2 - update
Change-Id: I3724f98d5755e764c5df50094e151bb0d445f5a0
</commit_message>
<xml_diff>
--- a/ctf/results/connectivity_benchmark_data.xlsx
+++ b/ctf/results/connectivity_benchmark_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raghu/Dropbox/workWithEdgar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{876660AE-2438-9549-AC19-E69327812032}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3A25D2-F331-CE41-A1C4-D9F6E7C21E97}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="520" windowWidth="27640" windowHeight="16540" xr2:uid="{0038F869-DDDC-FE49-9A78-7F5F6EEE82FE}"/>
   </bookViews>
@@ -273,8 +273,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="7"/>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:gradFill flip="none" rotWithShape="1">
                 <a:gsLst>
@@ -369,6 +369,12 @@
                 <c:pt idx="4">
                   <c:v>2.464</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.6150000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.8970000000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -414,13 +420,14 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="square"/>
-            <c:size val="7"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:gradFill flip="none" rotWithShape="1">
                 <a:gsLst>
@@ -513,6 +520,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>11.872</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.259</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45.494</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -726,7 +739,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -757,6 +770,7 @@
         <c:crossAx val="1053790336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1058019984"/>
@@ -1503,16 +1517,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>81280</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>797560</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>487680</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>40640</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1883,7 +1897,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2030,8 +2044,12 @@
         <f t="shared" si="0"/>
         <v>4194304</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="1">
+        <v>23.259</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4.6150000000000002</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -2047,8 +2065,12 @@
         <f t="shared" si="0"/>
         <v>8388608</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="1">
+        <v>45.494</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6.8970000000000002</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">

</xml_diff>